<commit_message>
Debug of Joints and Spring/Dampers
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/mcpherson_2d.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/mcpherson_2d.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B73BC5-CB55-4EC5-9861-99A88226D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6A3F14-D572-4C3A-9B0D-C34C53E0A3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="510" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="153">
   <si>
     <t>Mass</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Input T3 - Orientational Axis of Rot</t>
   </si>
   <si>
-    <t>Slider</t>
-  </si>
-  <si>
     <t>sp (global)</t>
   </si>
   <si>
@@ -299,15 +296,9 @@
     <t>Bodies ID</t>
   </si>
   <si>
-    <t>Crank</t>
-  </si>
-  <si>
     <t>Rot Ang [Rad]</t>
   </si>
   <si>
-    <t>Connecting Rod</t>
-  </si>
-  <si>
     <t>Units System</t>
   </si>
   <si>
@@ -384,9 +375,6 @@
   </si>
   <si>
     <t>mm*s^-2</t>
-  </si>
-  <si>
-    <t>mmks</t>
   </si>
   <si>
     <t>Linear - Spring Stiffness [N/mm]</t>
@@ -481,6 +469,39 @@
   </si>
   <si>
     <t>sj(REV axis) global</t>
+  </si>
+  <si>
+    <t>Sprung Mass</t>
+  </si>
+  <si>
+    <t>Control Arm</t>
+  </si>
+  <si>
+    <t>Unsprung Mass</t>
+  </si>
+  <si>
+    <t>K Tyre</t>
+  </si>
+  <si>
+    <t>K Primary</t>
+  </si>
+  <si>
+    <t>N Primary</t>
+  </si>
+  <si>
+    <t>N Tyre</t>
+  </si>
+  <si>
+    <t>Sprung - Control</t>
+  </si>
+  <si>
+    <t>Control - Unsprung</t>
+  </si>
+  <si>
+    <t>Sprung- Unsprung</t>
+  </si>
+  <si>
+    <t>mmks</t>
   </si>
 </sst>
 </file>
@@ -698,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -814,12 +835,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -829,9 +844,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -841,6 +853,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -868,28 +898,37 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -901,15 +940,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,6 +955,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -938,33 +1004,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1354,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25:J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,62 +1409,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58"/>
-      <c r="I2" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="55"/>
-      <c r="L2" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="M2" s="55"/>
-      <c r="O2" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="P2" s="53"/>
+      <c r="B2" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+      <c r="I2" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="58"/>
+      <c r="L2" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="58"/>
+      <c r="O2" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="60"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M3" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="O3" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="P3" s="50" t="s">
-        <v>137</v>
+        <v>100</v>
+      </c>
+      <c r="O3" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="30">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
@@ -1434,183 +1473,188 @@
         <v>0</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L4" s="38" t="s">
         <v>0</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="O4" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="50" t="s">
+      <c r="P4" s="47" t="s">
         <v>5</v>
       </c>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="I5" s="38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M5" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="P5" s="50" t="s">
-        <v>138</v>
+        <v>102</v>
+      </c>
+      <c r="O5" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="P5" s="47" t="s">
+        <v>134</v>
       </c>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30" t="s">
-        <v>82</v>
-      </c>
       <c r="I6" s="38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J6" s="38" t="s">
         <v>22</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="50" t="s">
+      <c r="O6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="50" t="s">
+      <c r="P6" s="47" t="s">
         <v>10</v>
       </c>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="30">
+        <f>-9.81*10^3</f>
+        <v>-9810</v>
+      </c>
       <c r="E7" s="35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M7" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="O7" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="50" t="s">
+      <c r="P7" s="47" t="s">
         <v>12</v>
       </c>
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="54"/>
+      <c r="B8" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="57"/>
       <c r="D8" s="30" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L8" s="38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M8" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="O8" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="O8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="P8" s="47" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="54"/>
+      <c r="B9" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="57"/>
       <c r="D9" s="30"/>
       <c r="E9" s="35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L9" s="39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="O9" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="O9" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="P9" s="50" t="s">
+      <c r="P9" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="O10" s="39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P10" s="39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="O11" s="39" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P11" s="39" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
@@ -1623,10 +1667,10 @@
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="O13" s="39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P13" s="39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -1639,10 +1683,10 @@
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="O15" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="P15" s="50" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="P15" s="47" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1668,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView topLeftCell="Q13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,125 +1732,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="62"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="55" t="s">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55" t="s">
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55" t="s">
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="58"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="64" t="s">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="68"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="S2" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>2</v>
@@ -1853,52 +1897,52 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="65"/>
-      <c r="S3" s="63"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="65"/>
       <c r="T3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="V3" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="W3" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="W3" s="29" t="s">
+      <c r="Y3" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="X3" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y3" s="29" t="s">
-        <v>68</v>
-      </c>
       <c r="Z3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AA3" s="29" t="s">
+      <c r="AB3" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AB3" s="29" t="s">
+      <c r="AC3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AC3" s="29" t="s">
+      <c r="AD3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="AD3" s="29" t="s">
+      <c r="AE3" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="AE3" s="29" t="s">
+      <c r="AF3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="AF3" s="29" t="s">
+      <c r="AG3" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AG3" s="29" t="s">
+      <c r="AH3" s="29" t="s">
         <v>61</v>
-      </c>
-      <c r="AH3" s="29" t="s">
-        <v>62</v>
       </c>
       <c r="AI3" s="34" t="s">
         <v>2</v>
@@ -2028,42 +2072,42 @@
         <v>2</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="C5" s="18">
-        <v>86.6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="17">
-        <v>-50</v>
+        <v>284.48</v>
       </c>
       <c r="E5" s="24">
         <v>0</v>
       </c>
-      <c r="F5" s="36">
-        <v>0</v>
-      </c>
-      <c r="G5" s="36">
-        <v>0</v>
-      </c>
-      <c r="H5" s="36">
-        <v>0</v>
-      </c>
-      <c r="I5" s="36">
-        <v>0</v>
-      </c>
-      <c r="J5" s="36">
-        <v>0</v>
-      </c>
-      <c r="K5" s="36">
-        <v>0</v>
-      </c>
-      <c r="L5" s="36">
-        <v>0</v>
-      </c>
-      <c r="M5" s="36">
-        <v>0</v>
-      </c>
-      <c r="N5" s="36">
+      <c r="F5" s="49">
+        <v>0</v>
+      </c>
+      <c r="G5" s="49">
+        <v>0</v>
+      </c>
+      <c r="H5" s="49">
+        <v>0</v>
+      </c>
+      <c r="I5" s="49">
+        <v>0</v>
+      </c>
+      <c r="J5" s="49">
+        <v>0</v>
+      </c>
+      <c r="K5" s="49">
+        <v>0</v>
+      </c>
+      <c r="L5" s="49">
+        <v>0</v>
+      </c>
+      <c r="M5" s="49">
+        <v>0</v>
+      </c>
+      <c r="N5" s="49">
         <v>0</v>
       </c>
       <c r="O5" s="36">
@@ -2073,39 +2117,40 @@
         <v>0</v>
       </c>
       <c r="Q5" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="36">
-        <v>-0.52359999999999995</v>
+        <v>0</v>
       </c>
       <c r="S5" s="17">
-        <v>0.33610000000000001</v>
+        <v>240</v>
       </c>
       <c r="T5" s="17">
-        <v>13.79</v>
+        <v>0</v>
       </c>
       <c r="U5" s="17">
-        <v>1304.74</v>
+        <v>0</v>
       </c>
       <c r="V5" s="17">
-        <v>1312.9336000000001</v>
-      </c>
-      <c r="W5" s="36">
-        <v>0</v>
-      </c>
-      <c r="X5" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="36">
+        <f>17.85*10^6</f>
+        <v>17850000</v>
+      </c>
+      <c r="W5" s="49">
+        <v>0</v>
+      </c>
+      <c r="X5" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="49">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="49">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="49">
         <v>0</v>
       </c>
       <c r="AC5" s="40">
@@ -2124,15 +2169,15 @@
         <v>0</v>
       </c>
       <c r="AH5" s="40">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="36">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="49">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="49">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="49">
         <v>0</v>
       </c>
     </row>
@@ -2141,42 +2186,42 @@
         <v>3</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="C6" s="18">
-        <v>418.1</v>
+        <v>274.19</v>
       </c>
       <c r="D6" s="17">
-        <v>-50</v>
+        <v>166.12</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="36">
-        <v>0</v>
-      </c>
-      <c r="G6" s="36">
-        <v>0</v>
-      </c>
-      <c r="H6" s="36">
-        <v>0</v>
-      </c>
-      <c r="I6" s="36">
-        <v>0</v>
-      </c>
-      <c r="J6" s="36">
-        <v>0</v>
-      </c>
-      <c r="K6" s="36">
-        <v>0</v>
-      </c>
-      <c r="L6" s="36">
-        <v>0</v>
-      </c>
-      <c r="M6" s="36">
-        <v>0</v>
-      </c>
-      <c r="N6" s="36">
+      <c r="F6" s="49">
+        <v>0</v>
+      </c>
+      <c r="G6" s="49">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49">
+        <v>0</v>
+      </c>
+      <c r="I6" s="49">
+        <v>0</v>
+      </c>
+      <c r="J6" s="49">
+        <v>0</v>
+      </c>
+      <c r="K6" s="49">
+        <v>0</v>
+      </c>
+      <c r="L6" s="49">
+        <v>0</v>
+      </c>
+      <c r="M6" s="49">
+        <v>0</v>
+      </c>
+      <c r="N6" s="49">
         <v>0</v>
       </c>
       <c r="O6" s="36">
@@ -2186,41 +2231,40 @@
         <v>0</v>
       </c>
       <c r="Q6" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="36">
-        <v>0.20100000000000001</v>
+        <v>0</v>
       </c>
       <c r="S6" s="17">
-        <v>5.2492999999999999</v>
+        <v>3</v>
       </c>
       <c r="T6" s="17">
-        <v>1345.9128000000001</v>
+        <v>0</v>
       </c>
       <c r="U6" s="17">
-        <f>1.27307*10^5</f>
-        <v>127306.99999999999</v>
+        <v>0</v>
       </c>
       <c r="V6" s="37">
-        <f>1.2810726*10^5</f>
-        <v>128107.26</v>
-      </c>
-      <c r="W6" s="36">
-        <v>0</v>
-      </c>
-      <c r="X6" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="36">
+        <f>0.03*10^6</f>
+        <v>30000</v>
+      </c>
+      <c r="W6" s="49">
+        <v>0</v>
+      </c>
+      <c r="X6" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="49">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="49">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="49">
         <v>0</v>
       </c>
       <c r="AC6" s="40">
@@ -2241,13 +2285,13 @@
       <c r="AH6" s="40">
         <v>0</v>
       </c>
-      <c r="AI6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="36">
+      <c r="AI6" s="49">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="49">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="49">
         <v>0</v>
       </c>
     </row>
@@ -2256,42 +2300,42 @@
         <v>4</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="C7" s="17">
-        <v>720</v>
+        <v>489.71</v>
       </c>
       <c r="D7" s="17">
-        <v>0</v>
+        <v>304.8</v>
       </c>
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="36">
-        <v>0</v>
-      </c>
-      <c r="G7" s="36">
-        <v>0</v>
-      </c>
-      <c r="H7" s="36">
-        <v>0</v>
-      </c>
-      <c r="I7" s="36">
-        <v>0</v>
-      </c>
-      <c r="J7" s="36">
-        <v>0</v>
-      </c>
-      <c r="K7" s="36">
-        <v>0</v>
-      </c>
-      <c r="L7" s="36">
-        <v>0</v>
-      </c>
-      <c r="M7" s="36">
-        <v>0</v>
-      </c>
-      <c r="N7" s="36">
+      <c r="F7" s="49">
+        <v>0</v>
+      </c>
+      <c r="G7" s="49">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49">
+        <v>0</v>
+      </c>
+      <c r="I7" s="49">
+        <v>0</v>
+      </c>
+      <c r="J7" s="49">
+        <v>0</v>
+      </c>
+      <c r="K7" s="49">
+        <v>0</v>
+      </c>
+      <c r="L7" s="49">
+        <v>0</v>
+      </c>
+      <c r="M7" s="49">
+        <v>0</v>
+      </c>
+      <c r="N7" s="49">
         <v>0</v>
       </c>
       <c r="O7" s="36">
@@ -2301,39 +2345,40 @@
         <v>0</v>
       </c>
       <c r="Q7" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="36">
-        <v>0</v>
+        <v>0.30387229999999998</v>
       </c>
       <c r="S7" s="17">
-        <v>2.9956</v>
+        <v>40</v>
       </c>
       <c r="T7" s="17">
-        <v>1997.056</v>
+        <v>0</v>
       </c>
       <c r="U7" s="17">
-        <v>3994.1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="17">
-        <v>5192.3455999999996</v>
-      </c>
-      <c r="W7" s="36">
-        <v>0</v>
-      </c>
-      <c r="X7" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="36">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="36">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="36">
+        <f>1.58*10^6</f>
+        <v>1580000</v>
+      </c>
+      <c r="W7" s="49">
+        <v>0</v>
+      </c>
+      <c r="X7" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="49">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="49">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="49">
         <v>0</v>
       </c>
       <c r="AC7" s="40">
@@ -2354,13 +2399,13 @@
       <c r="AH7" s="40">
         <v>0</v>
       </c>
-      <c r="AI7" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="36">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="36">
+      <c r="AI7" s="49">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="49">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="49">
         <v>0</v>
       </c>
     </row>
@@ -2385,15 +2430,15 @@
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2403,15 +2448,15 @@
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -2421,15 +2466,15 @@
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2463,6 +2508,9 @@
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2478,6 +2526,9 @@
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -5438,6 +5489,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -5451,12 +5508,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5465,10 +5516,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X64"/>
+  <dimension ref="A1:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26:N26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5485,16 +5536,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5525,11 +5576,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
+      <c r="F2" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5585,19 +5636,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
+      <c r="A5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -5623,12 +5674,12 @@
         <v>9</v>
       </c>
       <c r="F6" s="72" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="73"/>
       <c r="H6" s="74"/>
       <c r="I6" s="72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J6" s="73"/>
       <c r="K6" s="74"/>
@@ -5690,22 +5741,22 @@
       <c r="X8" s="10"/>
     </row>
     <row r="9" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -5730,21 +5781,21 @@
       <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="66" t="s">
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -5798,19 +5849,19 @@
       <c r="X12" s="10"/>
     </row>
     <row r="13" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -5835,16 +5886,16 @@
       <c r="E14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
+      <c r="F14" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
@@ -5854,17 +5905,43 @@
       <c r="X14" s="10"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="A15" s="21">
+        <v>1</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="21">
+        <v>2</v>
+      </c>
+      <c r="E15" s="21">
+        <v>3</v>
+      </c>
+      <c r="F15" s="23">
+        <f>0.122682*10^3</f>
+        <v>122.682</v>
+      </c>
+      <c r="G15" s="23">
+        <f>0.166116*10^3</f>
+        <v>166.11600000000001</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23">
+        <f>0.122682*10^3</f>
+        <v>122.682</v>
+      </c>
+      <c r="J15" s="23">
+        <f>0.166116*10^3</f>
+        <v>166.11600000000001</v>
+      </c>
+      <c r="K15" s="23">
+        <v>1</v>
+      </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
@@ -5874,17 +5951,43 @@
       <c r="X15" s="10"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="A16" s="14">
+        <v>2</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3</v>
+      </c>
+      <c r="E16" s="14">
+        <v>4</v>
+      </c>
+      <c r="F16" s="14">
+        <f>0.4257*10^3</f>
+        <v>425.70000000000005</v>
+      </c>
+      <c r="G16" s="14">
+        <f>0.166116*10^3</f>
+        <v>166.11600000000001</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0</v>
+      </c>
+      <c r="I16" s="50">
+        <f>0.4257*10^3</f>
+        <v>425.70000000000005</v>
+      </c>
+      <c r="J16" s="50">
+        <f>0.166116*10^3</f>
+        <v>166.11600000000001</v>
+      </c>
+      <c r="K16" s="50">
+        <v>1</v>
+      </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
@@ -5893,20 +5996,18 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
     </row>
-    <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -5915,81 +6016,81 @@
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
     </row>
-    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+    </row>
+    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="F19" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-    </row>
-    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="9"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-    </row>
-    <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+    </row>
+    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="9"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -5998,45 +6099,54 @@
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
     </row>
-    <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+    </row>
+    <row r="23" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C23" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="66" t="s">
+      <c r="F23" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-    </row>
-    <row r="23" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
     </row>
     <row r="24" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
@@ -6051,68 +6161,68 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:24" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
-      <c r="N25" s="67"/>
-    </row>
-    <row r="26" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+    <row r="25" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:24" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="69"/>
+    </row>
+    <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B27" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C27" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D27" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="49" t="s">
+      <c r="E27" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="68" t="s">
+      <c r="F27" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66" t="s">
-        <v>145</v>
-      </c>
-      <c r="M26" s="66"/>
-      <c r="N26" s="66"/>
-    </row>
-    <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="M27" s="71"/>
+      <c r="N27" s="71"/>
     </row>
     <row r="28" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
@@ -6127,173 +6237,212 @@
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:24" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="67" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="67"/>
-      <c r="N29" s="67"/>
-      <c r="O29" s="67"/>
-      <c r="P29" s="67"/>
-      <c r="Q29" s="67"/>
-    </row>
-    <row r="30" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+    <row r="29" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:24" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+    </row>
+    <row r="31" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B31" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C31" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E31" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="72" t="s">
+      <c r="F31" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="73"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="73"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="J30" s="73"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="M30" s="66"/>
-      <c r="N30" s="66"/>
-      <c r="O30" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="P30" s="66"/>
-      <c r="Q30" s="66"/>
-    </row>
-    <row r="31" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-    </row>
-    <row r="32" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="67" t="s">
+      <c r="J31" s="73"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+    </row>
+    <row r="32" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <v>3</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="21">
+        <v>2</v>
+      </c>
+      <c r="E32" s="21">
+        <v>4</v>
+      </c>
+      <c r="F32" s="23">
+        <f>0.26035*10^3</f>
+        <v>260.35000000000002</v>
+      </c>
+      <c r="G32" s="23">
+        <f>0.69342*10^3</f>
+        <v>693.42000000000007</v>
+      </c>
+      <c r="H32" s="23">
+        <v>0</v>
+      </c>
+      <c r="I32" s="23">
+        <f>0.41097*10^3</f>
+        <v>410.97</v>
+      </c>
+      <c r="J32" s="23">
+        <f>0.213084*10^3</f>
+        <v>213.084</v>
+      </c>
+      <c r="K32" s="23">
+        <v>0</v>
+      </c>
+      <c r="L32" s="19">
+        <f>0.26035*10^3</f>
+        <v>260.35000000000002</v>
+      </c>
+      <c r="M32" s="19">
+        <f>0.69342*10^3</f>
+        <v>693.42000000000007</v>
+      </c>
+      <c r="N32" s="19">
+        <v>1</v>
+      </c>
+      <c r="O32" s="19">
+        <f>0.230429*10^3</f>
+        <v>230.429</v>
+      </c>
+      <c r="P32" s="19">
+        <f>0.598002*10^3</f>
+        <v>598.00200000000007</v>
+      </c>
+      <c r="Q32" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="10"/>
-    </row>
-    <row r="34" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+    </row>
+    <row r="35" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B35" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C35" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D35" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-    </row>
-    <row r="35" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="9"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
-      <c r="W36" s="10"/>
-      <c r="X36" s="10"/>
-    </row>
-    <row r="37" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
+    <row r="36" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="9"/>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
@@ -6302,53 +6451,62 @@
       <c r="W37" s="10"/>
       <c r="X37" s="10"/>
     </row>
-    <row r="38" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+    </row>
+    <row r="39" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>1</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <v>1</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -6357,55 +6515,57 @@
       <c r="J40" s="11"/>
       <c r="K40" s="11"/>
     </row>
-    <row r="41" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="69" t="s">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+    </row>
+    <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="9"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="77"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-    </row>
-    <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
@@ -6426,12 +6586,10 @@
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
-      <c r="H45"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -6439,25 +6597,53 @@
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="M48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="64" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H46"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="65" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A25:N25"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="A30:Q30"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="A26:N26"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A9:N9"/>
@@ -6470,31 +6656,16 @@
     <mergeCell ref="A13:K13"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="I14:K14"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="A29:Q29"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Spherical,Universal,Revolute,Translation,Cylindrical,Simple,Ground,Driver"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52:B1038 B43:B46" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53:B1039 B44:B47" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Spherical,Universal,Revolute,Cylindrical,Translation,Simple,Driver,Ground,Point"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6509,7 +6680,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6523,18 +6694,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="A1" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -6550,18 +6721,18 @@
         <v>16</v>
       </c>
       <c r="E2" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6581,7 +6752,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -6601,10 +6772,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356001A-570B-4774-AE32-331534C6A696}">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6612,371 +6783,513 @@
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="9" max="9" width="36" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-    </row>
-    <row r="2" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="91" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="93"/>
-      <c r="R2" s="85" t="s">
-        <v>127</v>
-      </c>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+    </row>
+    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="91"/>
+      <c r="U2" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+    </row>
+    <row r="3" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="28" t="s">
+      <c r="F3" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="N3" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="O3" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="P3" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="K3" s="44" t="s">
-        <v>121</v>
-      </c>
-      <c r="L3" s="44" t="s">
+      <c r="Q3" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="N3" s="90" t="s">
-        <v>126</v>
-      </c>
-      <c r="O3" s="90"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R3" s="88"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="85"/>
-      <c r="W4" s="85"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="14">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14">
+        <v>4</v>
+      </c>
+      <c r="F4" s="50">
+        <f>0.26035*10^3</f>
+        <v>260.35000000000002</v>
+      </c>
+      <c r="G4" s="50">
+        <f>0.69342*10^3</f>
+        <v>693.42000000000007</v>
+      </c>
+      <c r="H4" s="50">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <f>0.41097*10^3</f>
+        <v>410.97</v>
+      </c>
+      <c r="J4" s="14">
+        <f>0.213084*10^3</f>
+        <v>213.084</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="32">
+        <f>140000*10^-3</f>
+        <v>140</v>
+      </c>
+      <c r="M4" s="41"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R6" s="85"/>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="85"/>
-      <c r="W6" s="85"/>
-    </row>
-    <row r="7" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
-    </row>
-    <row r="8" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="84"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="85"/>
-      <c r="W8" s="85"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="14">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="50">
+        <f>0.515112*10^3</f>
+        <v>515.11199999999997</v>
+      </c>
+      <c r="G5" s="50">
+        <f>0.3*10^3</f>
+        <v>300</v>
+      </c>
+      <c r="H5" s="50">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14">
+        <f>400000*10^-3</f>
+        <v>400</v>
+      </c>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="83"/>
+    </row>
+    <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="95" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+    </row>
+    <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="99"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="83"/>
+    </row>
+    <row r="9" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="28" t="s">
+      <c r="F9" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="93"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="P9" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="K9" s="48" t="s">
+      <c r="Q9" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="M9" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="N9" s="88" t="s">
-        <v>125</v>
-      </c>
-      <c r="O9" s="89"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R9" s="87"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="83"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="27"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="85"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="85"/>
-      <c r="V10" s="85"/>
-      <c r="W10" s="85"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="14">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4</v>
+      </c>
+      <c r="F10" s="51">
+        <f>0.26035*10^3</f>
+        <v>260.35000000000002</v>
+      </c>
+      <c r="G10" s="51">
+        <f>0.69342*10^3</f>
+        <v>693.42000000000007</v>
+      </c>
+      <c r="H10" s="51">
+        <v>0</v>
+      </c>
+      <c r="I10" s="51">
+        <f>0.41097*10^3</f>
+        <v>410.97</v>
+      </c>
+      <c r="J10" s="51">
+        <f>0.213084*10^3</f>
+        <v>213.084</v>
+      </c>
+      <c r="K10" s="51">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <f>6000*10^-3</f>
+        <v>6</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="83"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="85"/>
-      <c r="U11" s="85"/>
-      <c r="V11" s="85"/>
-      <c r="W11" s="85"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R12" s="85"/>
-      <c r="S12" s="85"/>
-      <c r="T12" s="85"/>
-      <c r="U12" s="85"/>
-      <c r="V12" s="85"/>
-      <c r="W12" s="85"/>
-    </row>
-    <row r="13" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="69" t="s">
+      <c r="B11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="14">
+        <v>4</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1</v>
+      </c>
+      <c r="F11" s="51">
+        <f>0.515112*10^3</f>
+        <v>515.11199999999997</v>
+      </c>
+      <c r="G11" s="51">
+        <f>0.3*10^3</f>
+        <v>300</v>
+      </c>
+      <c r="H11" s="51">
+        <v>0</v>
+      </c>
+      <c r="I11" s="51">
+        <v>0</v>
+      </c>
+      <c r="J11" s="51">
+        <v>0</v>
+      </c>
+      <c r="K11" s="51">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <f>10000*10^-3</f>
+        <v>10</v>
+      </c>
+      <c r="U11" s="83"/>
+      <c r="V11" s="83"/>
+      <c r="W11" s="83"/>
+      <c r="X11" s="83"/>
+      <c r="Y11" s="83"/>
+      <c r="Z11" s="83"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U12" s="83"/>
+      <c r="V12" s="83"/>
+      <c r="W12" s="83"/>
+      <c r="X12" s="83"/>
+      <c r="Y12" s="83"/>
+      <c r="Z12" s="83"/>
+    </row>
+    <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="76"/>
+      <c r="O13" s="76"/>
+      <c r="P13" s="76"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="U13" s="83"/>
+      <c r="V13" s="83"/>
+      <c r="W13" s="83"/>
+      <c r="X13" s="83"/>
+      <c r="Y13" s="83"/>
+      <c r="Z13" s="83"/>
+    </row>
+    <row r="14" spans="1:26" s="45" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="84"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="71"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="85"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
-      <c r="W13" s="85"/>
-    </row>
-    <row r="14" spans="1:23" s="47" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="86" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -6985,16 +7298,19 @@
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -7003,24 +7319,29 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="R2:W13"/>
+  <mergeCells count="17">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="A7:R7"/>
+    <mergeCell ref="U2:Z13"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="M14:O14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="A13:P13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="J2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7031,16 +7352,16 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J18:J19"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="94"/>
+      <c r="A2" s="100" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>